<commit_message>
updates budget and adds bluetooth test sketch
</commit_message>
<xml_diff>
--- a/prototypes/second_iteration/budget.xlsx
+++ b/prototypes/second_iteration/budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\diy-ventilator\prototypes\second_iteration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906D766F-C169-4DCF-87B9-31677B7A8A9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1D1552-A9AE-4917-A0F1-62E840CA5178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{98A0F2A8-A92E-4AD8-8DB8-2CF3193E3003}"/>
   </bookViews>
@@ -140,12 +140,6 @@
     <t>SODIAL®</t>
   </si>
   <si>
-    <t>9CR0612H001</t>
-  </si>
-  <si>
-    <t>Sanyo Denki America</t>
-  </si>
-  <si>
     <t>Wires + Misc</t>
   </si>
   <si>
@@ -168,6 +162,12 @@
   </si>
   <si>
     <t>Approximate Weight (kg)</t>
+  </si>
+  <si>
+    <t>STEADY MOTOR</t>
+  </si>
+  <si>
+    <t>WM7040-24V</t>
   </si>
 </sst>
 </file>
@@ -312,6 +312,27 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -369,27 +390,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -404,15 +404,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C29CA1C1-CAE2-48E7-B815-07AF7CC4E533}" name="Table1" displayName="Table1" ref="A4:F15" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C29CA1C1-CAE2-48E7-B815-07AF7CC4E533}" name="Table1" displayName="Table1" ref="A4:F15" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A4:F15" xr:uid="{FFE9C588-F5B8-4752-B8B6-0A2DF7F3324C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{723464C2-6E89-4A12-BE88-1DDD9DCF4367}" name="Part Name"/>
     <tableColumn id="2" xr3:uid="{DECAF936-EC34-4D3D-879D-8427B61A9850}" name="Manufacturer"/>
     <tableColumn id="3" xr3:uid="{385A877C-9A07-46EA-BD46-419D8E9E1A4A}" name="Part Number"/>
-    <tableColumn id="4" xr3:uid="{1403C813-B548-450C-B6DB-0F49D44DD949}" name="Price" dataDxfId="5" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{1403C813-B548-450C-B6DB-0F49D44DD949}" name="Price" dataDxfId="4" dataCellStyle="Currency"/>
     <tableColumn id="5" xr3:uid="{8CD5C559-1966-46D1-9DFE-692C76C652FA}" name="Quantity Needed"/>
-    <tableColumn id="6" xr3:uid="{FF5F3308-AE9E-4259-B8F9-1EB3C5A8E05A}" name="Total" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{FF5F3308-AE9E-4259-B8F9-1EB3C5A8E05A}" name="Total" dataDxfId="3">
       <calculatedColumnFormula>D5*E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -421,15 +421,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0F845197-75B7-4D83-BCC7-45B7CDA2BE27}" name="Table3" displayName="Table3" ref="A18:F21" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0F845197-75B7-4D83-BCC7-45B7CDA2BE27}" name="Table3" displayName="Table3" ref="A18:F21" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A18:F21" xr:uid="{8063FF08-10E2-4AFB-AC6B-74F1C1A116FC}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{34287877-A948-4F8D-9E03-49F7ABAF4ADC}" name="Part Name"/>
     <tableColumn id="2" xr3:uid="{8C94812D-66FE-4A53-814A-4B76BB88F5DD}" name="Manufacturer"/>
     <tableColumn id="3" xr3:uid="{51E18B0D-6634-47E9-8328-B85C92558A71}" name="Part Number"/>
-    <tableColumn id="4" xr3:uid="{FEDAC801-F9E4-478E-B97B-02A544C9D39A}" name="Avg Filament Price (per kg)" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{FEDAC801-F9E4-478E-B97B-02A544C9D39A}" name="Avg Filament Price (per kg)" dataDxfId="1" dataCellStyle="Currency"/>
     <tableColumn id="5" xr3:uid="{89E59625-C494-4C7B-982B-DAE10E744E2E}" name="Approximate Weight (kg)"/>
-    <tableColumn id="6" xr3:uid="{A7651E66-5913-444D-A18B-E5B215FC40F6}" name="Total" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{A7651E66-5913-444D-A18B-E5B215FC40F6}" name="Total" dataDxfId="0">
       <calculatedColumnFormula>D19*E19</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -737,7 +737,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F1" s="9">
         <f xml:space="preserve"> SUM(F5:F22)</f>
@@ -835,10 +835,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2">
         <v>45</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2">
         <v>20</v>
@@ -1011,10 +1011,10 @@
         <v>9</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>17</v>
@@ -1025,10 +1025,10 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>25</v>
@@ -1046,10 +1046,10 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
         <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
       </c>
       <c r="D20" s="2">
         <v>25</v>
@@ -1067,10 +1067,10 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2">
         <v>25</v>

</xml_diff>